<commit_message>
dowload files with px_last p1
</commit_message>
<xml_diff>
--- a/files_creation/data/input/fields.xlsx
+++ b/files_creation/data/input/fields.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33606\OneDrive - EDHEC\Desktop\Trading\SI\Stats_SI\files_creation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33606\OneDrive - EDHEC\Desktop\Trading\SI\Stats_SI\files_creation\data\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5644AD7-A6B8-48D7-972F-469CE9215A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C0A1FB8-E92A-41CB-A3BD-94C054884F43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43967636-AB28-48D4-B48C-4285AEE8A4E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{43967636-AB28-48D4-B48C-4285AEE8A4E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="123">
   <si>
     <t>PX707</t>
   </si>
@@ -399,6 +399,15 @@
   </si>
   <si>
     <t>FLDS_Description</t>
+  </si>
+  <si>
+    <t>PR005</t>
+  </si>
+  <si>
+    <t>PX_LAST</t>
+  </si>
+  <si>
+    <t>Last Price</t>
   </si>
 </sst>
 </file>
@@ -759,10 +768,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EE1AF641-3358-4E74-B4AC-AA5880B16AB7}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1256,6 +1265,17 @@
         <v>116</v>
       </c>
     </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>120</v>
+      </c>
+      <c r="B45" t="s">
+        <v>121</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:C44" xr:uid="{EE1AF641-3358-4E74-B4AC-AA5880B16AB7}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>